<commit_message>
added code YAML version, fixed bugs
</commit_message>
<xml_diff>
--- a/python_results.xlsx
+++ b/python_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,220 +441,119 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Which keyword is used to define a variable in Python?</t>
+          <t>What is the standard algorithm for inserting an item into a sorted array?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None of the above</t>
+          <t>Insertion sort</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>None of the above</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Insertion sort</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>What is the output of this code: print(2 + 3 * 4)</t>
+          <t>What is a sequential file?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>Sequential file is a file that stores data in a sequential manner.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Sequential file is a file that stores data in a sequential manner.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Which method is used to add an element to the end of a list in Python?</t>
+          <t>What is the standard algorithm for sorting an array?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>append()</t>
+          <t>Selection sort</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>append()</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Selection sort</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Which keyword is used to exit a loop in Python?</t>
+          <t>What is the standard algorithm for deleting an item from a sorted array?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>continue</t>
+          <t>Deletion sort</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>break</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Deletion sort</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Which data structure is used to store a collection of key-value pairs in Python?</t>
+          <t>What is the standard algorithm for appending to a sequential file?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>dictionary</t>
+          <t>OPEN and WRITE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dictionary</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>OPEN and WRITE</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>What is the keyword used to define a function in Python?</t>
+          <t>What is the standard algorithm for searching an unsorted array?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>define</t>
+          <t>Binary search</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>def</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Linear search</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Which loop is used to iterate over a sequence of elements in Python?</t>
+          <t>What is the difference between a sequential file and a relative file?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>repeat-until</t>
+          <t>Sequential files can only be read from beginning to end, while relative files can be read from any point.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>for</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Which operator is used to perform exponentiation in Python?</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>**</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>**</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>What is the output of this code: print('Hello, world!')[::-1]</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>'dlrow ,olleH'</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>'!dlrow ,olleH'</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Which data type is used to store a sequence of characters in Python?</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Sequential files can only be read from beginning to end, while relative files can be read from any point.</t>
         </is>
       </c>
     </row>

</xml_diff>